<commit_message>
hiv works a treat
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_hiv.xlsx
+++ b/tests/databooks/databook_hiv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1C5AD0E1-D8F4-4F4B-9DD8-FA0302F97206}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{415FE31B-E96C-3640-A70A-852BF266BFE0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="640" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -194,6 +194,7 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,7 +872,7 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1346,10 +1347,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1360,7 +1361,7 @@
     <col min="4" max="4" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>females</v>
@@ -1400,7 +1401,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>males</v>
@@ -1419,7 +1420,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>females</v>
@@ -1458,7 +1459,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>males</v>
@@ -1476,7 +1477,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>females</v>
@@ -1515,8 +1516,9 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>males</v>
@@ -1535,7 +1537,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1556,7 +1558,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>females</v>
@@ -1574,7 +1576,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>males</v>

</xml_diff>

<commit_message>
add simple tb frw
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_hiv.xlsx
+++ b/tests/databooks/databook_hiv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{415FE31B-E96C-3640-A70A-852BF266BFE0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9EEABE87-CF5B-ED41-A3E5-B843689C3A81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="640" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0\ _k_r_._-;\-* #,##0\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +114,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -176,10 +187,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,8 +207,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
@@ -828,7 +844,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -872,8 +888,8 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -882,6 +898,7 @@
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="3.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -917,7 +934,7 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="7">
         <v>3390000</v>
       </c>
       <c r="F2" s="2"/>
@@ -935,7 +952,7 @@
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="7">
         <v>2540000</v>
       </c>
       <c r="F3" s="2"/>
@@ -1350,7 +1367,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E6" sqref="E6:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>